<commit_message>
File & folder cache working, still have some bugs to fix
</commit_message>
<xml_diff>
--- a/test/data/Substrate/P0097B_20250721160205.xlsx
+++ b/test/data/Substrate/P0097B_20250721160205.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CFA88F-1C0A-C241-ACC7-4A33EBA0B8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D386A6BF-9509-468F-AACC-8F5477F879EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="5880" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -730,16 +730,16 @@
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34">
+    <row r="1" spans="1:4" ht="27.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Wafer map DB load success.
</commit_message>
<xml_diff>
--- a/test/data/Substrate/P0097B_20250721160205.xlsx
+++ b/test/data/Substrate/P0097B_20250721160205.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D386A6BF-9509-468F-AACC-8F5477F879EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2131179-09E4-4102-BFD4-C81ED5AD50FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4642" yWindow="3555" windowWidth="21601" windowHeight="12683" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="129">
   <si>
     <t>Product ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -346,6 +346,75 @@
   </si>
   <si>
     <t>86107919CNF1</t>
+  </si>
+  <si>
+    <t>86809619CNG7</t>
+  </si>
+  <si>
+    <t>65420204CNF0</t>
+  </si>
+  <si>
+    <t>63518033CNC5</t>
+  </si>
+  <si>
+    <t>63617427CNF6</t>
+  </si>
+  <si>
+    <t>65220505CNC7</t>
+  </si>
+  <si>
+    <t>18009303CNC5</t>
+  </si>
+  <si>
+    <t>75119936CNC7</t>
+  </si>
+  <si>
+    <t>79817714CNA4</t>
+  </si>
+  <si>
+    <t>71319718CNG7</t>
+  </si>
+  <si>
+    <t>61016332CNH2</t>
+  </si>
+  <si>
+    <t>73716819CNC3</t>
+  </si>
+  <si>
+    <t>66316625CNF0</t>
+  </si>
+  <si>
+    <t>84207528CNC7</t>
+  </si>
+  <si>
+    <t>62317612CNB7</t>
+  </si>
+  <si>
+    <t>70819903CND2</t>
+  </si>
+  <si>
+    <t>75320025CNF3</t>
+  </si>
+  <si>
+    <t>62117517CNF4</t>
+  </si>
+  <si>
+    <t>75719206CNG6</t>
+  </si>
+  <si>
+    <t>72119624CNG4</t>
+  </si>
+  <si>
+    <t>73818504CNE0</t>
+  </si>
+  <si>
+    <t>82408825CNF7</t>
+  </si>
+  <si>
+    <t>63617406CNH2</t>
+  </si>
+  <si>
+    <t>63617408CNB0</t>
   </si>
 </sst>
 </file>
@@ -435,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -447,6 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +800,7 @@
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
@@ -763,8 +833,8 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>105</v>
+      <c r="D2" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -791,8 +861,8 @@
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>105</v>
+      <c r="D4" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -805,8 +875,8 @@
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>105</v>
+      <c r="D5" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -819,8 +889,8 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>105</v>
+      <c r="D6" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -833,8 +903,8 @@
       <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>105</v>
+      <c r="D7" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -847,8 +917,8 @@
       <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>105</v>
+      <c r="D8" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -861,8 +931,8 @@
       <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>105</v>
+      <c r="D9" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -875,8 +945,8 @@
       <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>105</v>
+      <c r="D10" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -889,8 +959,8 @@
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>105</v>
+      <c r="D11" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -903,8 +973,8 @@
       <c r="C12" s="2">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>105</v>
+      <c r="D12" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -917,8 +987,8 @@
       <c r="C13" s="2">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>105</v>
+      <c r="D13" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -931,8 +1001,8 @@
       <c r="C14" s="2">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>105</v>
+      <c r="D14" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -945,8 +1015,8 @@
       <c r="C15" s="2">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>105</v>
+      <c r="D15" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -959,8 +1029,8 @@
       <c r="C16" s="2">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>105</v>
+      <c r="D16" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -973,8 +1043,8 @@
       <c r="C17" s="2">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>105</v>
+      <c r="D17" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -987,8 +1057,8 @@
       <c r="C18" s="2">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>105</v>
+      <c r="D18" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1001,8 +1071,8 @@
       <c r="C19" s="2">
         <v>18</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>105</v>
+      <c r="D19" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1015,8 +1085,8 @@
       <c r="C20" s="2">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>105</v>
+      <c r="D20" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1029,8 +1099,8 @@
       <c r="C21" s="2">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>105</v>
+      <c r="D21" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1043,8 +1113,8 @@
       <c r="C22" s="2">
         <v>21</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>105</v>
+      <c r="D22" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1057,8 +1127,8 @@
       <c r="C23" s="2">
         <v>22</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>105</v>
+      <c r="D23" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1071,8 +1141,8 @@
       <c r="C24" s="2">
         <v>23</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>105</v>
+      <c r="D24" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1085,8 +1155,8 @@
       <c r="C25" s="2">
         <v>24</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>105</v>
+      <c r="D25" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4">

</xml_diff>